<commit_message>
updating music sources list
</commit_message>
<xml_diff>
--- a/src/assets/ChatTrinityMusicSourceData.xlsx
+++ b/src/assets/ChatTrinityMusicSourceData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter\Vivo Music Dropbox\Trinity College London\TCL National\Strategy &amp; R&amp;D\R&amp;D\Chatbot\Source Data\Music\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3164B74E-32C2-4C71-81E7-3AEBC91C9C3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC3E46CB-8C56-4165-935B-A3AA105BFD74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{767CB8E1-717A-4A4B-9A2F-73181A3DE1DB}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$B$211</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$B$216</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="223">
   <si>
     <t>Web/PDF</t>
   </si>
@@ -676,6 +676,27 @@
   </si>
   <si>
     <t>Jazz Woodwind online Jan 2023 (7383)</t>
+  </si>
+  <si>
+    <t>Trinity Music Performance Diplomas Syllabus (8556)</t>
+  </si>
+  <si>
+    <t>Diplomas in Music Teaching Syllabus (4001)</t>
+  </si>
+  <si>
+    <t>Music Theory Diplomas Syllabus (7382)</t>
+  </si>
+  <si>
+    <t>Bariton_Euphonium_Diplomas_Jan2022 (8531)</t>
+  </si>
+  <si>
+    <t>Guitar_Diplomas_Jan2022 (8539)</t>
+  </si>
+  <si>
+    <t>https://resources.trinitycollege.com/performance-diplomas/programme-notes-for-ftcl</t>
+  </si>
+  <si>
+    <t>https://www.trinitycollege.com/qualifications/music/diplomas/performance/resources/written-programmes-ATCL-LTCL</t>
   </si>
 </sst>
 </file>
@@ -1036,7 +1057,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50C14BDF-EED2-4551-A2A9-086DD03AE42C}">
-  <dimension ref="A1:B213"/>
+  <dimension ref="A1:B220"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1056,762 +1077,762 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>204</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>179</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>219</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>211</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>207</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>184</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>165</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>148</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>202</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>172</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>161</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>128</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
+        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
+        <v>118</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>126</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B22" t="s">
-        <v>22</v>
+        <v>140</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B23" t="s">
-        <v>23</v>
+        <v>114</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B24" t="s">
-        <v>24</v>
+        <v>144</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B25" t="s">
-        <v>25</v>
+        <v>112</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B26" t="s">
-        <v>26</v>
+        <v>160</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B27" t="s">
-        <v>27</v>
+        <v>99</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B28" t="s">
-        <v>28</v>
+        <v>132</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B29" t="s">
-        <v>29</v>
+        <v>106</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B30" t="s">
-        <v>30</v>
+        <v>108</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B31" t="s">
-        <v>31</v>
+        <v>185</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B32" t="s">
-        <v>32</v>
+        <v>109</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B33" t="s">
-        <v>33</v>
+        <v>101</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B34" t="s">
-        <v>34</v>
+        <v>105</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B35" t="s">
-        <v>35</v>
+        <v>103</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B36" t="s">
-        <v>36</v>
+        <v>115</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B37" t="s">
-        <v>37</v>
+        <v>121</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B38" t="s">
-        <v>38</v>
+        <v>217</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B39" t="s">
-        <v>39</v>
+        <v>198</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B40" t="s">
-        <v>40</v>
+        <v>203</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B41" t="s">
-        <v>41</v>
+        <v>138</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B42" t="s">
-        <v>42</v>
+        <v>173</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B43" t="s">
-        <v>43</v>
+        <v>157</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B44" t="s">
-        <v>44</v>
+        <v>110</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B45" t="s">
-        <v>45</v>
+        <v>145</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B46" t="s">
-        <v>46</v>
+        <v>155</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B47" t="s">
-        <v>47</v>
+        <v>147</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B48" t="s">
-        <v>48</v>
+        <v>116</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B49" t="s">
-        <v>49</v>
+        <v>194</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B50" t="s">
-        <v>50</v>
+        <v>205</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B51" t="s">
-        <v>51</v>
+        <v>134</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B52" t="s">
-        <v>52</v>
+        <v>220</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B53" t="s">
-        <v>53</v>
+        <v>189</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B54" t="s">
-        <v>54</v>
+        <v>206</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B55" t="s">
-        <v>55</v>
+        <v>201</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B56" t="s">
-        <v>56</v>
+        <v>98</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B57" t="s">
-        <v>57</v>
+        <v>186</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B58" t="s">
-        <v>58</v>
+        <v>100</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B59" t="s">
-        <v>59</v>
+        <v>215</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B60" t="s">
-        <v>60</v>
+        <v>183</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B61" t="s">
-        <v>61</v>
+        <v>190</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B62" t="s">
-        <v>62</v>
+        <v>146</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B63" t="s">
-        <v>63</v>
+        <v>135</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B64" t="s">
-        <v>64</v>
+        <v>218</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B65" t="s">
-        <v>65</v>
+        <v>119</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B66" t="s">
-        <v>66</v>
+        <v>162</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B67" t="s">
-        <v>67</v>
+        <v>175</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B68" t="s">
-        <v>68</v>
+        <v>196</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B69" t="s">
-        <v>69</v>
+        <v>163</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B70" t="s">
-        <v>70</v>
+        <v>174</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B71" t="s">
-        <v>71</v>
+        <v>197</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B72" t="s">
-        <v>72</v>
+        <v>187</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B73" t="s">
-        <v>73</v>
+        <v>193</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B74" t="s">
-        <v>74</v>
+        <v>107</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B75" t="s">
-        <v>75</v>
+        <v>212</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B76" t="s">
-        <v>76</v>
+        <v>102</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B77" t="s">
-        <v>77</v>
+        <v>104</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B78" t="s">
-        <v>78</v>
+        <v>152</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B79" t="s">
-        <v>79</v>
+        <v>182</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B80" t="s">
-        <v>80</v>
+        <v>143</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B81" t="s">
-        <v>81</v>
+        <v>166</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B82" t="s">
-        <v>82</v>
+        <v>168</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B83" t="s">
-        <v>83</v>
+        <v>122</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B84" t="s">
-        <v>84</v>
+        <v>180</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B85" t="s">
-        <v>85</v>
+        <v>159</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B86" t="s">
-        <v>86</v>
+        <v>169</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B87" t="s">
-        <v>87</v>
+        <v>154</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B88" t="s">
-        <v>88</v>
+        <v>156</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B89" t="s">
-        <v>89</v>
+        <v>149</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B90" t="s">
-        <v>90</v>
+        <v>142</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B91" t="s">
-        <v>91</v>
+        <v>153</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B92" t="s">
-        <v>92</v>
+        <v>139</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B93" t="s">
-        <v>93</v>
+        <v>170</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B94" t="s">
-        <v>94</v>
+        <v>158</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B95" t="s">
-        <v>95</v>
+        <v>167</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="B96" t="s">
-        <v>96</v>
+        <v>171</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.45">
@@ -1819,7 +1840,7 @@
         <v>213</v>
       </c>
       <c r="B97" t="s">
-        <v>98</v>
+        <v>123</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.45">
@@ -1827,7 +1848,7 @@
         <v>213</v>
       </c>
       <c r="B98" t="s">
-        <v>99</v>
+        <v>131</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.45">
@@ -1835,7 +1856,7 @@
         <v>213</v>
       </c>
       <c r="B99" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.45">
@@ -1843,7 +1864,7 @@
         <v>213</v>
       </c>
       <c r="B100" t="s">
-        <v>101</v>
+        <v>210</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.45">
@@ -1851,7 +1872,7 @@
         <v>213</v>
       </c>
       <c r="B101" t="s">
-        <v>102</v>
+        <v>192</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.45">
@@ -1859,7 +1880,7 @@
         <v>213</v>
       </c>
       <c r="B102" t="s">
-        <v>103</v>
+        <v>150</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.45">
@@ -1867,7 +1888,7 @@
         <v>213</v>
       </c>
       <c r="B103" t="s">
-        <v>104</v>
+        <v>191</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.45">
@@ -1875,7 +1896,7 @@
         <v>213</v>
       </c>
       <c r="B104" t="s">
-        <v>105</v>
+        <v>164</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.45">
@@ -1883,7 +1904,7 @@
         <v>213</v>
       </c>
       <c r="B105" t="s">
-        <v>106</v>
+        <v>177</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.45">
@@ -1891,7 +1912,7 @@
         <v>213</v>
       </c>
       <c r="B106" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.45">
@@ -1899,7 +1920,7 @@
         <v>213</v>
       </c>
       <c r="B107" t="s">
-        <v>108</v>
+        <v>216</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.45">
@@ -1907,7 +1928,7 @@
         <v>213</v>
       </c>
       <c r="B108" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.45">
@@ -1915,7 +1936,7 @@
         <v>213</v>
       </c>
       <c r="B109" t="s">
-        <v>110</v>
+        <v>130</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.45">
@@ -1923,7 +1944,7 @@
         <v>213</v>
       </c>
       <c r="B110" t="s">
-        <v>111</v>
+        <v>151</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.45">
@@ -1931,7 +1952,7 @@
         <v>213</v>
       </c>
       <c r="B111" t="s">
-        <v>112</v>
+        <v>136</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.45">
@@ -1939,7 +1960,7 @@
         <v>213</v>
       </c>
       <c r="B112" t="s">
-        <v>113</v>
+        <v>195</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.45">
@@ -1947,7 +1968,7 @@
         <v>213</v>
       </c>
       <c r="B113" t="s">
-        <v>114</v>
+        <v>199</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.45">
@@ -1955,7 +1976,7 @@
         <v>213</v>
       </c>
       <c r="B114" t="s">
-        <v>115</v>
+        <v>181</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.45">
@@ -1963,7 +1984,7 @@
         <v>213</v>
       </c>
       <c r="B115" t="s">
-        <v>116</v>
+        <v>176</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.45">
@@ -1971,7 +1992,7 @@
         <v>213</v>
       </c>
       <c r="B116" t="s">
-        <v>117</v>
+        <v>208</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.45">
@@ -1979,7 +2000,7 @@
         <v>213</v>
       </c>
       <c r="B117" t="s">
-        <v>118</v>
+        <v>209</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.45">
@@ -1987,7 +2008,7 @@
         <v>213</v>
       </c>
       <c r="B118" t="s">
-        <v>119</v>
+        <v>200</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.45">
@@ -1995,7 +2016,7 @@
         <v>213</v>
       </c>
       <c r="B119" t="s">
-        <v>120</v>
+        <v>178</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.45">
@@ -2003,7 +2024,7 @@
         <v>213</v>
       </c>
       <c r="B120" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.45">
@@ -2011,7 +2032,7 @@
         <v>213</v>
       </c>
       <c r="B121" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.45">
@@ -2019,7 +2040,7 @@
         <v>213</v>
       </c>
       <c r="B122" t="s">
-        <v>123</v>
+        <v>214</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.45">
@@ -2027,731 +2048,791 @@
         <v>213</v>
       </c>
       <c r="B123" t="s">
-        <v>124</v>
+        <v>141</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A124" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B124" t="s">
-        <v>125</v>
+        <v>2</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A125" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B125" t="s">
-        <v>126</v>
+        <v>3</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A126" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B126" t="s">
-        <v>127</v>
+        <v>4</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A127" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B127" t="s">
-        <v>128</v>
+        <v>5</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A128" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B128" t="s">
-        <v>129</v>
+        <v>6</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A129" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B129" t="s">
-        <v>130</v>
+        <v>7</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A130" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B130" t="s">
-        <v>131</v>
+        <v>8</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A131" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B131" t="s">
-        <v>132</v>
+        <v>9</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A132" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B132" t="s">
-        <v>133</v>
+        <v>10</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A133" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B133" t="s">
-        <v>134</v>
+        <v>11</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A134" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B134" t="s">
-        <v>135</v>
+        <v>12</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A135" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B135" t="s">
-        <v>136</v>
+        <v>13</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A136" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B136" t="s">
-        <v>137</v>
+        <v>14</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A137" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B137" t="s">
-        <v>138</v>
+        <v>15</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A138" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B138" t="s">
-        <v>139</v>
+        <v>16</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A139" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B139" t="s">
-        <v>140</v>
+        <v>17</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A140" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B140" t="s">
-        <v>141</v>
+        <v>18</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A141" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B141" t="s">
-        <v>142</v>
+        <v>19</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A142" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B142" t="s">
-        <v>143</v>
+        <v>20</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A143" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B143" t="s">
-        <v>144</v>
+        <v>21</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A144" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B144" t="s">
-        <v>145</v>
+        <v>22</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A145" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B145" t="s">
-        <v>146</v>
+        <v>23</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A146" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B146" t="s">
-        <v>147</v>
+        <v>24</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A147" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B147" t="s">
-        <v>148</v>
+        <v>25</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A148" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B148" t="s">
-        <v>149</v>
+        <v>26</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A149" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B149" t="s">
-        <v>150</v>
+        <v>27</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A150" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B150" t="s">
-        <v>151</v>
+        <v>28</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A151" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B151" t="s">
-        <v>152</v>
+        <v>29</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A152" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B152" t="s">
-        <v>153</v>
+        <v>30</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A153" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B153" t="s">
-        <v>154</v>
+        <v>31</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A154" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B154" t="s">
-        <v>155</v>
+        <v>32</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A155" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B155" t="s">
-        <v>156</v>
+        <v>33</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A156" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B156" t="s">
-        <v>157</v>
+        <v>34</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A157" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B157" t="s">
-        <v>158</v>
+        <v>35</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A158" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B158" t="s">
-        <v>159</v>
+        <v>36</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A159" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B159" t="s">
-        <v>160</v>
+        <v>37</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A160" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B160" t="s">
-        <v>161</v>
+        <v>38</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A161" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B161" t="s">
-        <v>162</v>
+        <v>39</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A162" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B162" t="s">
-        <v>163</v>
+        <v>40</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A163" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B163" t="s">
-        <v>164</v>
+        <v>41</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A164" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B164" t="s">
-        <v>165</v>
+        <v>42</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A165" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B165" t="s">
-        <v>166</v>
+        <v>43</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A166" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B166" t="s">
-        <v>167</v>
+        <v>44</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A167" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B167" t="s">
-        <v>168</v>
+        <v>45</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A168" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B168" t="s">
-        <v>169</v>
+        <v>46</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A169" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B169" t="s">
-        <v>170</v>
+        <v>47</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A170" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B170" t="s">
-        <v>171</v>
+        <v>48</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A171" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B171" t="s">
-        <v>172</v>
+        <v>49</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A172" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B172" t="s">
-        <v>173</v>
+        <v>50</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A173" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B173" t="s">
-        <v>174</v>
+        <v>51</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A174" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B174" t="s">
-        <v>175</v>
+        <v>52</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A175" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B175" t="s">
-        <v>176</v>
+        <v>53</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A176" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B176" t="s">
-        <v>177</v>
+        <v>54</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A177" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B177" t="s">
-        <v>178</v>
+        <v>55</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A178" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B178" t="s">
-        <v>179</v>
+        <v>56</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A179" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B179" t="s">
-        <v>180</v>
+        <v>57</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A180" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B180" t="s">
-        <v>181</v>
+        <v>58</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A181" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B181" t="s">
-        <v>182</v>
+        <v>59</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A182" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B182" t="s">
-        <v>183</v>
+        <v>60</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A183" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B183" t="s">
-        <v>184</v>
+        <v>61</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A184" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B184" t="s">
-        <v>185</v>
+        <v>62</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A185" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B185" t="s">
-        <v>186</v>
+        <v>63</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A186" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B186" t="s">
-        <v>187</v>
+        <v>64</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A187" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B187" t="s">
-        <v>188</v>
+        <v>65</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A188" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B188" t="s">
-        <v>189</v>
+        <v>66</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A189" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B189" t="s">
-        <v>190</v>
+        <v>67</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A190" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B190" t="s">
-        <v>191</v>
+        <v>68</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A191" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B191" t="s">
-        <v>192</v>
+        <v>69</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A192" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B192" t="s">
-        <v>193</v>
+        <v>70</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A193" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B193" t="s">
-        <v>194</v>
+        <v>71</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A194" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B194" t="s">
-        <v>195</v>
+        <v>72</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A195" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B195" t="s">
-        <v>196</v>
+        <v>73</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A196" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B196" t="s">
-        <v>197</v>
+        <v>74</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A197" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B197" t="s">
-        <v>198</v>
+        <v>75</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A198" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B198" t="s">
-        <v>199</v>
+        <v>76</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A199" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B199" t="s">
-        <v>200</v>
+        <v>77</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A200" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B200" t="s">
-        <v>201</v>
+        <v>78</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A201" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B201" t="s">
-        <v>202</v>
+        <v>79</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A202" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B202" t="s">
-        <v>203</v>
+        <v>80</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A203" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B203" t="s">
-        <v>204</v>
+        <v>81</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A204" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B204" t="s">
-        <v>205</v>
+        <v>221</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A205" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B205" t="s">
-        <v>206</v>
+        <v>82</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A206" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B206" t="s">
-        <v>207</v>
+        <v>83</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A207" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B207" t="s">
-        <v>208</v>
+        <v>84</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A208" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B208" t="s">
-        <v>209</v>
+        <v>85</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A209" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B209" t="s">
-        <v>210</v>
+        <v>86</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A210" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B210" t="s">
-        <v>211</v>
+        <v>87</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A211" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B211" t="s">
-        <v>212</v>
+        <v>88</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A212" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B212" t="s">
-        <v>215</v>
+        <v>89</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A213" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B213" t="s">
-        <v>214</v>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A214" t="s">
+        <v>97</v>
+      </c>
+      <c r="B214" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A215" t="s">
+        <v>97</v>
+      </c>
+      <c r="B215" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A216" t="s">
+        <v>97</v>
+      </c>
+      <c r="B216" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A217" t="s">
+        <v>97</v>
+      </c>
+      <c r="B217" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A218" t="s">
+        <v>97</v>
+      </c>
+      <c r="B218" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A219" t="s">
+        <v>97</v>
+      </c>
+      <c r="B219" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A220" t="s">
+        <v>97</v>
+      </c>
+      <c r="B220" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B211" xr:uid="{50C14BDF-EED2-4551-A2A9-086DD03AE42C}"/>
+  <autoFilter ref="A1:B216" xr:uid="{50C14BDF-EED2-4551-A2A9-086DD03AE42C}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B220">
+    <sortCondition ref="A2:A220"/>
+    <sortCondition ref="B2:B220"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update music data sources
</commit_message>
<xml_diff>
--- a/src/assets/ChatTrinityMusicSourceData.xlsx
+++ b/src/assets/ChatTrinityMusicSourceData.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter\Vivo Music Dropbox\Trinity College London\TCL National\Strategy &amp; R&amp;D\R&amp;D\Chatbot\Source Data\Music\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter\Vivo Music Dropbox\Trinity College London\TCL National\Strategy &amp; R&amp;D\R&amp;D\Chatbot\Code\ChatTrinity\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC3E46CB-8C56-4165-935B-A3AA105BFD74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55742691-BF26-4F47-928E-8DF7FB956EB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{767CB8E1-717A-4A4B-9A2F-73181A3DE1DB}"/>
+    <workbookView xWindow="8" yWindow="8" windowWidth="22485" windowHeight="14385" xr2:uid="{767CB8E1-717A-4A4B-9A2F-73181A3DE1DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$B$216</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$B$220</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -375,9 +375,6 @@
     <t>DGD Technical Work Classical Guitar (9181)</t>
   </si>
   <si>
-    <t>Digital Grades Step-by-Step Guide (UK) (9851)</t>
-  </si>
-  <si>
     <t>Flute_Nov-2022 (9979)</t>
   </si>
   <si>
@@ -570,9 +567,6 @@
     <t>AMusTCL Reading List (713)</t>
   </si>
   <si>
-    <t>Singing 2018-2023 syllabus (10036)</t>
-  </si>
-  <si>
     <t>Trumpet repertoire lists (8882)</t>
   </si>
   <si>
@@ -697,6 +691,12 @@
   </si>
   <si>
     <t>https://www.trinitycollege.com/qualifications/music/diplomas/performance/resources/written-programmes-ATCL-LTCL</t>
+  </si>
+  <si>
+    <t>Singing syllabus 2023 (7929)</t>
+  </si>
+  <si>
+    <t>https://www.trinitycollege.com/qualifications/digital/digital-grades-diplomas/recorded-accompaniments-for-digital-grade-music-exams</t>
   </si>
 </sst>
 </file>
@@ -1059,7 +1059,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50C14BDF-EED2-4551-A2A9-086DD03AE42C}">
   <dimension ref="A1:B220"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -1077,175 +1079,175 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B8" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B9" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B11" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B13" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B15" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B16" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B17" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B19" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B21" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B23" t="s">
         <v>114</v>
@@ -1253,15 +1255,15 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B24" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B25" t="s">
         <v>112</v>
@@ -1269,15 +1271,15 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B26" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B27" t="s">
         <v>99</v>
@@ -1285,15 +1287,15 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B28" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B29" t="s">
         <v>106</v>
@@ -1301,7 +1303,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B30" t="s">
         <v>108</v>
@@ -1309,15 +1311,15 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B31" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B32" t="s">
         <v>109</v>
@@ -1325,7 +1327,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B33" t="s">
         <v>101</v>
@@ -1333,7 +1335,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B34" t="s">
         <v>105</v>
@@ -1341,7 +1343,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B35" t="s">
         <v>103</v>
@@ -1349,706 +1351,706 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B36" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B37" t="s">
-        <v>121</v>
+        <v>215</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B38" t="s">
-        <v>217</v>
+        <v>196</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B39" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B40" t="s">
-        <v>203</v>
+        <v>137</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B41" t="s">
-        <v>138</v>
+        <v>172</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B42" t="s">
-        <v>173</v>
+        <v>156</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B43" t="s">
-        <v>157</v>
+        <v>110</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B44" t="s">
-        <v>110</v>
+        <v>144</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B45" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B46" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B47" t="s">
-        <v>147</v>
+        <v>115</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B48" t="s">
-        <v>116</v>
+        <v>192</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B49" t="s">
-        <v>194</v>
+        <v>203</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B50" t="s">
-        <v>205</v>
+        <v>133</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B51" t="s">
-        <v>134</v>
+        <v>218</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B52" t="s">
-        <v>220</v>
+        <v>187</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B53" t="s">
-        <v>189</v>
+        <v>204</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B54" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B55" t="s">
-        <v>201</v>
+        <v>98</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B56" t="s">
-        <v>98</v>
+        <v>184</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B57" t="s">
-        <v>186</v>
+        <v>100</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
+        <v>211</v>
+      </c>
+      <c r="B58" t="s">
         <v>213</v>
-      </c>
-      <c r="B58" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B59" t="s">
-        <v>215</v>
+        <v>181</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B60" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B61" t="s">
-        <v>190</v>
+        <v>145</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B62" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B63" t="s">
-        <v>135</v>
+        <v>216</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B64" t="s">
-        <v>218</v>
+        <v>118</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B65" t="s">
-        <v>119</v>
+        <v>161</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B66" t="s">
-        <v>162</v>
+        <v>174</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B67" t="s">
-        <v>175</v>
+        <v>194</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B68" t="s">
-        <v>196</v>
+        <v>162</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B69" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B70" t="s">
-        <v>174</v>
+        <v>195</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B71" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B72" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B73" t="s">
-        <v>193</v>
+        <v>107</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B74" t="s">
-        <v>107</v>
+        <v>210</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B75" t="s">
-        <v>212</v>
+        <v>102</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B76" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B77" t="s">
-        <v>104</v>
+        <v>151</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B78" t="s">
-        <v>152</v>
+        <v>180</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B79" t="s">
-        <v>182</v>
+        <v>142</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B80" t="s">
-        <v>143</v>
+        <v>165</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B81" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B82" t="s">
-        <v>168</v>
+        <v>121</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B83" t="s">
-        <v>122</v>
+        <v>221</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B84" t="s">
-        <v>180</v>
+        <v>158</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B85" t="s">
-        <v>159</v>
+        <v>168</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B86" t="s">
-        <v>169</v>
+        <v>153</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B87" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B88" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B89" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B90" t="s">
-        <v>142</v>
+        <v>152</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B91" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B92" t="s">
-        <v>139</v>
+        <v>169</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B93" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B94" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B95" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B96" t="s">
-        <v>171</v>
+        <v>122</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B97" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B98" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B99" t="s">
-        <v>113</v>
+        <v>208</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B100" t="s">
-        <v>210</v>
+        <v>190</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B101" t="s">
-        <v>192</v>
+        <v>149</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A102" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B102" t="s">
-        <v>150</v>
+        <v>189</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A103" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B103" t="s">
-        <v>191</v>
+        <v>163</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A104" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B104" t="s">
-        <v>164</v>
+        <v>176</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A105" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B105" t="s">
-        <v>177</v>
+        <v>111</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A106" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B106" t="s">
-        <v>111</v>
+        <v>214</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A107" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B107" t="s">
-        <v>216</v>
+        <v>116</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A108" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B108" t="s">
-        <v>117</v>
+        <v>129</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A109" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B109" t="s">
-        <v>130</v>
+        <v>150</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A110" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B110" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A111" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B111" t="s">
-        <v>136</v>
+        <v>193</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A112" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B112" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A113" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B113" t="s">
-        <v>199</v>
+        <v>179</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A114" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B114" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A115" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B115" t="s">
-        <v>176</v>
+        <v>206</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A116" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B116" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A117" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B117" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A118" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B118" t="s">
-        <v>200</v>
+        <v>177</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A119" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B119" t="s">
-        <v>178</v>
+        <v>136</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A120" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B120" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A121" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B121" t="s">
-        <v>124</v>
+        <v>212</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A122" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B122" t="s">
-        <v>214</v>
+        <v>140</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A123" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="B123" t="s">
-        <v>141</v>
+        <v>2</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.45">
@@ -2056,7 +2058,7 @@
         <v>97</v>
       </c>
       <c r="B124" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.45">
@@ -2064,7 +2066,7 @@
         <v>97</v>
       </c>
       <c r="B125" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.45">
@@ -2072,7 +2074,7 @@
         <v>97</v>
       </c>
       <c r="B126" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.45">
@@ -2080,7 +2082,7 @@
         <v>97</v>
       </c>
       <c r="B127" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.45">
@@ -2088,7 +2090,7 @@
         <v>97</v>
       </c>
       <c r="B128" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.45">
@@ -2096,7 +2098,7 @@
         <v>97</v>
       </c>
       <c r="B129" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.45">
@@ -2104,7 +2106,7 @@
         <v>97</v>
       </c>
       <c r="B130" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.45">
@@ -2112,7 +2114,7 @@
         <v>97</v>
       </c>
       <c r="B131" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.45">
@@ -2120,7 +2122,7 @@
         <v>97</v>
       </c>
       <c r="B132" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.45">
@@ -2128,7 +2130,7 @@
         <v>97</v>
       </c>
       <c r="B133" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.45">
@@ -2136,7 +2138,7 @@
         <v>97</v>
       </c>
       <c r="B134" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.45">
@@ -2144,7 +2146,7 @@
         <v>97</v>
       </c>
       <c r="B135" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.45">
@@ -2152,7 +2154,7 @@
         <v>97</v>
       </c>
       <c r="B136" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.45">
@@ -2160,7 +2162,7 @@
         <v>97</v>
       </c>
       <c r="B137" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.45">
@@ -2168,7 +2170,7 @@
         <v>97</v>
       </c>
       <c r="B138" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.45">
@@ -2176,7 +2178,7 @@
         <v>97</v>
       </c>
       <c r="B139" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.45">
@@ -2184,7 +2186,7 @@
         <v>97</v>
       </c>
       <c r="B140" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.45">
@@ -2192,7 +2194,7 @@
         <v>97</v>
       </c>
       <c r="B141" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.45">
@@ -2200,7 +2202,7 @@
         <v>97</v>
       </c>
       <c r="B142" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.45">
@@ -2208,7 +2210,7 @@
         <v>97</v>
       </c>
       <c r="B143" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.45">
@@ -2216,7 +2218,7 @@
         <v>97</v>
       </c>
       <c r="B144" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.45">
@@ -2224,7 +2226,7 @@
         <v>97</v>
       </c>
       <c r="B145" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.45">
@@ -2232,7 +2234,7 @@
         <v>97</v>
       </c>
       <c r="B146" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.45">
@@ -2240,7 +2242,7 @@
         <v>97</v>
       </c>
       <c r="B147" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.45">
@@ -2248,7 +2250,7 @@
         <v>97</v>
       </c>
       <c r="B148" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.45">
@@ -2256,7 +2258,7 @@
         <v>97</v>
       </c>
       <c r="B149" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.45">
@@ -2264,7 +2266,7 @@
         <v>97</v>
       </c>
       <c r="B150" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.45">
@@ -2272,7 +2274,7 @@
         <v>97</v>
       </c>
       <c r="B151" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.45">
@@ -2280,7 +2282,7 @@
         <v>97</v>
       </c>
       <c r="B152" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.45">
@@ -2288,7 +2290,7 @@
         <v>97</v>
       </c>
       <c r="B153" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.45">
@@ -2296,7 +2298,7 @@
         <v>97</v>
       </c>
       <c r="B154" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.45">
@@ -2304,7 +2306,7 @@
         <v>97</v>
       </c>
       <c r="B155" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.45">
@@ -2312,7 +2314,7 @@
         <v>97</v>
       </c>
       <c r="B156" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.45">
@@ -2320,7 +2322,7 @@
         <v>97</v>
       </c>
       <c r="B157" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.45">
@@ -2328,7 +2330,7 @@
         <v>97</v>
       </c>
       <c r="B158" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.45">
@@ -2336,7 +2338,7 @@
         <v>97</v>
       </c>
       <c r="B159" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.45">
@@ -2344,7 +2346,7 @@
         <v>97</v>
       </c>
       <c r="B160" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.45">
@@ -2352,7 +2354,7 @@
         <v>97</v>
       </c>
       <c r="B161" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.45">
@@ -2360,7 +2362,7 @@
         <v>97</v>
       </c>
       <c r="B162" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.45">
@@ -2368,7 +2370,7 @@
         <v>97</v>
       </c>
       <c r="B163" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.45">
@@ -2376,7 +2378,7 @@
         <v>97</v>
       </c>
       <c r="B164" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.45">
@@ -2384,7 +2386,7 @@
         <v>97</v>
       </c>
       <c r="B165" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.45">
@@ -2392,7 +2394,7 @@
         <v>97</v>
       </c>
       <c r="B166" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.45">
@@ -2400,7 +2402,7 @@
         <v>97</v>
       </c>
       <c r="B167" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.45">
@@ -2408,7 +2410,7 @@
         <v>97</v>
       </c>
       <c r="B168" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.45">
@@ -2416,7 +2418,7 @@
         <v>97</v>
       </c>
       <c r="B169" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.45">
@@ -2424,7 +2426,7 @@
         <v>97</v>
       </c>
       <c r="B170" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.45">
@@ -2432,7 +2434,7 @@
         <v>97</v>
       </c>
       <c r="B171" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.45">
@@ -2440,7 +2442,7 @@
         <v>97</v>
       </c>
       <c r="B172" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.45">
@@ -2448,7 +2450,7 @@
         <v>97</v>
       </c>
       <c r="B173" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.45">
@@ -2456,7 +2458,7 @@
         <v>97</v>
       </c>
       <c r="B174" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.45">
@@ -2464,7 +2466,7 @@
         <v>97</v>
       </c>
       <c r="B175" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.45">
@@ -2472,7 +2474,7 @@
         <v>97</v>
       </c>
       <c r="B176" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.45">
@@ -2480,7 +2482,7 @@
         <v>97</v>
       </c>
       <c r="B177" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.45">
@@ -2488,7 +2490,7 @@
         <v>97</v>
       </c>
       <c r="B178" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.45">
@@ -2496,7 +2498,7 @@
         <v>97</v>
       </c>
       <c r="B179" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.45">
@@ -2504,7 +2506,7 @@
         <v>97</v>
       </c>
       <c r="B180" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.45">
@@ -2512,7 +2514,7 @@
         <v>97</v>
       </c>
       <c r="B181" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.45">
@@ -2520,7 +2522,7 @@
         <v>97</v>
       </c>
       <c r="B182" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.45">
@@ -2528,7 +2530,7 @@
         <v>97</v>
       </c>
       <c r="B183" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.45">
@@ -2536,7 +2538,7 @@
         <v>97</v>
       </c>
       <c r="B184" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.45">
@@ -2544,7 +2546,7 @@
         <v>97</v>
       </c>
       <c r="B185" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.45">
@@ -2552,7 +2554,7 @@
         <v>97</v>
       </c>
       <c r="B186" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.45">
@@ -2560,7 +2562,7 @@
         <v>97</v>
       </c>
       <c r="B187" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.45">
@@ -2568,7 +2570,7 @@
         <v>97</v>
       </c>
       <c r="B188" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.45">
@@ -2576,7 +2578,7 @@
         <v>97</v>
       </c>
       <c r="B189" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.45">
@@ -2584,7 +2586,7 @@
         <v>97</v>
       </c>
       <c r="B190" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.45">
@@ -2592,7 +2594,7 @@
         <v>97</v>
       </c>
       <c r="B191" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.45">
@@ -2600,7 +2602,7 @@
         <v>97</v>
       </c>
       <c r="B192" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.45">
@@ -2608,7 +2610,7 @@
         <v>97</v>
       </c>
       <c r="B193" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.45">
@@ -2616,7 +2618,7 @@
         <v>97</v>
       </c>
       <c r="B194" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.45">
@@ -2624,7 +2626,7 @@
         <v>97</v>
       </c>
       <c r="B195" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.45">
@@ -2632,7 +2634,7 @@
         <v>97</v>
       </c>
       <c r="B196" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.45">
@@ -2640,7 +2642,7 @@
         <v>97</v>
       </c>
       <c r="B197" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.45">
@@ -2648,7 +2650,7 @@
         <v>97</v>
       </c>
       <c r="B198" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.45">
@@ -2656,7 +2658,7 @@
         <v>97</v>
       </c>
       <c r="B199" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.45">
@@ -2664,7 +2666,7 @@
         <v>97</v>
       </c>
       <c r="B200" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.45">
@@ -2672,7 +2674,7 @@
         <v>97</v>
       </c>
       <c r="B201" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.45">
@@ -2680,7 +2682,7 @@
         <v>97</v>
       </c>
       <c r="B202" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.45">
@@ -2688,7 +2690,7 @@
         <v>97</v>
       </c>
       <c r="B203" t="s">
-        <v>81</v>
+        <v>219</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.45">
@@ -2696,7 +2698,7 @@
         <v>97</v>
       </c>
       <c r="B204" t="s">
-        <v>221</v>
+        <v>82</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.45">
@@ -2704,7 +2706,7 @@
         <v>97</v>
       </c>
       <c r="B205" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.45">
@@ -2712,7 +2714,7 @@
         <v>97</v>
       </c>
       <c r="B206" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.45">
@@ -2720,7 +2722,7 @@
         <v>97</v>
       </c>
       <c r="B207" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.45">
@@ -2728,7 +2730,7 @@
         <v>97</v>
       </c>
       <c r="B208" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.45">
@@ -2736,7 +2738,7 @@
         <v>97</v>
       </c>
       <c r="B209" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.45">
@@ -2744,7 +2746,7 @@
         <v>97</v>
       </c>
       <c r="B210" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.45">
@@ -2752,7 +2754,7 @@
         <v>97</v>
       </c>
       <c r="B211" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.45">
@@ -2760,7 +2762,7 @@
         <v>97</v>
       </c>
       <c r="B212" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.45">
@@ -2768,7 +2770,7 @@
         <v>97</v>
       </c>
       <c r="B213" t="s">
-        <v>90</v>
+        <v>220</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.45">
@@ -2776,7 +2778,7 @@
         <v>97</v>
       </c>
       <c r="B214" t="s">
-        <v>222</v>
+        <v>91</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.45">
@@ -2784,7 +2786,7 @@
         <v>97</v>
       </c>
       <c r="B215" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.45">
@@ -2792,7 +2794,7 @@
         <v>97</v>
       </c>
       <c r="B216" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.45">
@@ -2800,7 +2802,7 @@
         <v>97</v>
       </c>
       <c r="B217" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.45">
@@ -2808,7 +2810,7 @@
         <v>97</v>
       </c>
       <c r="B218" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.45">
@@ -2816,7 +2818,7 @@
         <v>97</v>
       </c>
       <c r="B219" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.45">
@@ -2824,14 +2826,14 @@
         <v>97</v>
       </c>
       <c r="B220" t="s">
-        <v>96</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B216" xr:uid="{50C14BDF-EED2-4551-A2A9-086DD03AE42C}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B220">
-    <sortCondition ref="A2:A220"/>
-    <sortCondition ref="B2:B220"/>
+  <autoFilter ref="A1:B220" xr:uid="{50C14BDF-EED2-4551-A2A9-086DD03AE42C}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B219">
+    <sortCondition ref="A2:A219"/>
+    <sortCondition ref="B2:B219"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update piano syllabus pdfs
</commit_message>
<xml_diff>
--- a/src/assets/ChatTrinityMusicSourceData.xlsx
+++ b/src/assets/ChatTrinityMusicSourceData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter\Vivo Music Dropbox\Trinity College London\TCL National\Strategy &amp; R&amp;D\R&amp;D\Chatbot\Code\ChatTrinity\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2198AF5D-2CDE-4E8D-8D42-DB4FFAAF86AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6817DF83-BEBB-471D-9F91-B2B4D75C2D7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{767CB8E1-717A-4A4B-9A2F-73181A3DE1DB}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$B$220</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$B$221</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="227">
   <si>
     <t>Web/PDF</t>
   </si>
@@ -700,13 +700,22 @@
   </si>
   <si>
     <t>https://www.trinitycollege.com/about-us/work-with-trinity/registered-exam-centre</t>
+  </si>
+  <si>
+    <t>Replaced 5/9/23 by "Piano F2F syllabus_ONLINE (9079).pdf"</t>
+  </si>
+  <si>
+    <t>Piano Syllabus Digital assessment (10127)</t>
+  </si>
+  <si>
+    <t>Piano F2F syllabus_ONLINE (9079)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -726,6 +735,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -752,10 +769,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1071,9 +1089,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50C14BDF-EED2-4551-A2A9-086DD03AE42C}">
-  <dimension ref="A1:B221"/>
+  <dimension ref="A1:C223"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A198" workbookViewId="0">
+      <selection activeCell="B218" sqref="B218"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -1593,7 +1613,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>211</v>
       </c>
@@ -1601,7 +1621,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>211</v>
       </c>
@@ -1609,7 +1629,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
         <v>211</v>
       </c>
@@ -1617,7 +1637,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>211</v>
       </c>
@@ -1625,7 +1645,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>211</v>
       </c>
@@ -1633,7 +1653,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>211</v>
       </c>
@@ -1641,7 +1661,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
         <v>211</v>
       </c>
@@ -1649,7 +1669,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
         <v>211</v>
       </c>
@@ -1657,68 +1677,71 @@
         <v>191</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
         <v>211</v>
       </c>
       <c r="B73" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A74" t="s">
+        <v>211</v>
+      </c>
+      <c r="B74" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A74" t="s">
-        <v>211</v>
-      </c>
-      <c r="B74" t="s">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A75" t="s">
+        <v>211</v>
+      </c>
+      <c r="B75" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A75" t="s">
-        <v>211</v>
-      </c>
-      <c r="B75" t="s">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A76" t="s">
+        <v>211</v>
+      </c>
+      <c r="B76" s="3" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A76" t="s">
-        <v>211</v>
-      </c>
-      <c r="B76" t="s">
+      <c r="C76" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A77" t="s">
+        <v>211</v>
+      </c>
+      <c r="B77" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A78" t="s">
+        <v>211</v>
+      </c>
+      <c r="B78" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A77" t="s">
-        <v>211</v>
-      </c>
-      <c r="B77" t="s">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A79" t="s">
+        <v>211</v>
+      </c>
+      <c r="B79" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A78" t="s">
-        <v>211</v>
-      </c>
-      <c r="B78" t="s">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A80" t="s">
+        <v>211</v>
+      </c>
+      <c r="B80" t="s">
         <v>180</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A79" t="s">
-        <v>211</v>
-      </c>
-      <c r="B79" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A80" t="s">
-        <v>211</v>
-      </c>
-      <c r="B80" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.45">
@@ -1726,7 +1749,7 @@
         <v>211</v>
       </c>
       <c r="B81" t="s">
-        <v>167</v>
+        <v>142</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.45">
@@ -1734,7 +1757,7 @@
         <v>211</v>
       </c>
       <c r="B82" t="s">
-        <v>121</v>
+        <v>165</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.45">
@@ -1742,7 +1765,7 @@
         <v>211</v>
       </c>
       <c r="B83" t="s">
-        <v>221</v>
+        <v>167</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.45">
@@ -1750,7 +1773,7 @@
         <v>211</v>
       </c>
       <c r="B84" t="s">
-        <v>158</v>
+        <v>121</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.45">
@@ -1758,7 +1781,7 @@
         <v>211</v>
       </c>
       <c r="B85" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.45">
@@ -1766,7 +1789,7 @@
         <v>211</v>
       </c>
       <c r="B86" t="s">
-        <v>153</v>
+        <v>168</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.45">
@@ -1774,7 +1797,7 @@
         <v>211</v>
       </c>
       <c r="B87" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.45">
@@ -1782,7 +1805,7 @@
         <v>211</v>
       </c>
       <c r="B88" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.45">
@@ -1790,7 +1813,7 @@
         <v>211</v>
       </c>
       <c r="B89" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.45">
@@ -1798,7 +1821,7 @@
         <v>211</v>
       </c>
       <c r="B90" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.45">
@@ -1806,7 +1829,7 @@
         <v>211</v>
       </c>
       <c r="B91" t="s">
-        <v>138</v>
+        <v>152</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.45">
@@ -1814,7 +1837,7 @@
         <v>211</v>
       </c>
       <c r="B92" t="s">
-        <v>169</v>
+        <v>138</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.45">
@@ -1822,7 +1845,7 @@
         <v>211</v>
       </c>
       <c r="B93" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.45">
@@ -1830,7 +1853,7 @@
         <v>211</v>
       </c>
       <c r="B94" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.45">
@@ -1838,7 +1861,7 @@
         <v>211</v>
       </c>
       <c r="B95" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.45">
@@ -1846,7 +1869,7 @@
         <v>211</v>
       </c>
       <c r="B96" t="s">
-        <v>122</v>
+        <v>170</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.45">
@@ -1854,7 +1877,7 @@
         <v>211</v>
       </c>
       <c r="B97" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.45">
@@ -1862,7 +1885,7 @@
         <v>211</v>
       </c>
       <c r="B98" t="s">
-        <v>113</v>
+        <v>221</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.45">
@@ -1870,7 +1893,7 @@
         <v>211</v>
       </c>
       <c r="B99" t="s">
-        <v>208</v>
+        <v>130</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.45">
@@ -1878,7 +1901,7 @@
         <v>211</v>
       </c>
       <c r="B100" t="s">
-        <v>190</v>
+        <v>113</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.45">
@@ -1886,7 +1909,7 @@
         <v>211</v>
       </c>
       <c r="B101" t="s">
-        <v>149</v>
+        <v>208</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.45">
@@ -1894,7 +1917,7 @@
         <v>211</v>
       </c>
       <c r="B102" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.45">
@@ -1902,7 +1925,7 @@
         <v>211</v>
       </c>
       <c r="B103" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.45">
@@ -1910,7 +1933,7 @@
         <v>211</v>
       </c>
       <c r="B104" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.45">
@@ -1918,7 +1941,7 @@
         <v>211</v>
       </c>
       <c r="B105" t="s">
-        <v>111</v>
+        <v>163</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.45">
@@ -1926,7 +1949,7 @@
         <v>211</v>
       </c>
       <c r="B106" t="s">
-        <v>214</v>
+        <v>176</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.45">
@@ -1934,7 +1957,7 @@
         <v>211</v>
       </c>
       <c r="B107" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.45">
@@ -1942,7 +1965,7 @@
         <v>211</v>
       </c>
       <c r="B108" t="s">
-        <v>129</v>
+        <v>214</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.45">
@@ -1950,7 +1973,7 @@
         <v>211</v>
       </c>
       <c r="B109" t="s">
-        <v>150</v>
+        <v>116</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.45">
@@ -1958,7 +1981,7 @@
         <v>211</v>
       </c>
       <c r="B110" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.45">
@@ -1966,7 +1989,7 @@
         <v>211</v>
       </c>
       <c r="B111" t="s">
-        <v>193</v>
+        <v>150</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.45">
@@ -1974,7 +1997,7 @@
         <v>211</v>
       </c>
       <c r="B112" t="s">
-        <v>197</v>
+        <v>135</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.45">
@@ -1982,7 +2005,7 @@
         <v>211</v>
       </c>
       <c r="B113" t="s">
-        <v>179</v>
+        <v>193</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.45">
@@ -1990,7 +2013,7 @@
         <v>211</v>
       </c>
       <c r="B114" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.45">
@@ -1998,7 +2021,7 @@
         <v>211</v>
       </c>
       <c r="B115" t="s">
-        <v>206</v>
+        <v>179</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.45">
@@ -2006,7 +2029,7 @@
         <v>211</v>
       </c>
       <c r="B116" t="s">
-        <v>207</v>
+        <v>175</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.45">
@@ -2014,7 +2037,7 @@
         <v>211</v>
       </c>
       <c r="B117" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.45">
@@ -2022,7 +2045,7 @@
         <v>211</v>
       </c>
       <c r="B118" t="s">
-        <v>177</v>
+        <v>207</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.45">
@@ -2030,7 +2053,7 @@
         <v>211</v>
       </c>
       <c r="B119" t="s">
-        <v>136</v>
+        <v>198</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.45">
@@ -2038,7 +2061,7 @@
         <v>211</v>
       </c>
       <c r="B120" t="s">
-        <v>123</v>
+        <v>177</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.45">
@@ -2046,7 +2069,7 @@
         <v>211</v>
       </c>
       <c r="B121" t="s">
-        <v>212</v>
+        <v>136</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.45">
@@ -2054,23 +2077,23 @@
         <v>211</v>
       </c>
       <c r="B122" t="s">
-        <v>140</v>
+        <v>123</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A123" t="s">
-        <v>97</v>
+        <v>211</v>
       </c>
       <c r="B123" t="s">
-        <v>2</v>
+        <v>212</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A124" t="s">
-        <v>97</v>
+        <v>211</v>
       </c>
       <c r="B124" t="s">
-        <v>3</v>
+        <v>140</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.45">
@@ -2078,7 +2101,7 @@
         <v>97</v>
       </c>
       <c r="B125" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.45">
@@ -2086,7 +2109,7 @@
         <v>97</v>
       </c>
       <c r="B126" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.45">
@@ -2094,7 +2117,7 @@
         <v>97</v>
       </c>
       <c r="B127" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.45">
@@ -2102,7 +2125,7 @@
         <v>97</v>
       </c>
       <c r="B128" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.45">
@@ -2110,7 +2133,7 @@
         <v>97</v>
       </c>
       <c r="B129" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.45">
@@ -2118,7 +2141,7 @@
         <v>97</v>
       </c>
       <c r="B130" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.45">
@@ -2126,7 +2149,7 @@
         <v>97</v>
       </c>
       <c r="B131" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.45">
@@ -2134,7 +2157,7 @@
         <v>97</v>
       </c>
       <c r="B132" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.45">
@@ -2142,7 +2165,7 @@
         <v>97</v>
       </c>
       <c r="B133" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.45">
@@ -2150,7 +2173,7 @@
         <v>97</v>
       </c>
       <c r="B134" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.45">
@@ -2158,7 +2181,7 @@
         <v>97</v>
       </c>
       <c r="B135" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.45">
@@ -2166,7 +2189,7 @@
         <v>97</v>
       </c>
       <c r="B136" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.45">
@@ -2174,7 +2197,7 @@
         <v>97</v>
       </c>
       <c r="B137" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.45">
@@ -2182,7 +2205,7 @@
         <v>97</v>
       </c>
       <c r="B138" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.45">
@@ -2190,7 +2213,7 @@
         <v>97</v>
       </c>
       <c r="B139" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.45">
@@ -2198,7 +2221,7 @@
         <v>97</v>
       </c>
       <c r="B140" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.45">
@@ -2206,7 +2229,7 @@
         <v>97</v>
       </c>
       <c r="B141" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.45">
@@ -2214,7 +2237,7 @@
         <v>97</v>
       </c>
       <c r="B142" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.45">
@@ -2222,7 +2245,7 @@
         <v>97</v>
       </c>
       <c r="B143" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.45">
@@ -2230,7 +2253,7 @@
         <v>97</v>
       </c>
       <c r="B144" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.45">
@@ -2238,7 +2261,7 @@
         <v>97</v>
       </c>
       <c r="B145" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.45">
@@ -2246,7 +2269,7 @@
         <v>97</v>
       </c>
       <c r="B146" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.45">
@@ -2254,7 +2277,7 @@
         <v>97</v>
       </c>
       <c r="B147" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.45">
@@ -2262,7 +2285,7 @@
         <v>97</v>
       </c>
       <c r="B148" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.45">
@@ -2270,7 +2293,7 @@
         <v>97</v>
       </c>
       <c r="B149" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.45">
@@ -2278,7 +2301,7 @@
         <v>97</v>
       </c>
       <c r="B150" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.45">
@@ -2286,7 +2309,7 @@
         <v>97</v>
       </c>
       <c r="B151" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.45">
@@ -2294,7 +2317,7 @@
         <v>97</v>
       </c>
       <c r="B152" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.45">
@@ -2302,7 +2325,7 @@
         <v>97</v>
       </c>
       <c r="B153" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.45">
@@ -2310,7 +2333,7 @@
         <v>97</v>
       </c>
       <c r="B154" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.45">
@@ -2318,7 +2341,7 @@
         <v>97</v>
       </c>
       <c r="B155" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.45">
@@ -2326,7 +2349,7 @@
         <v>97</v>
       </c>
       <c r="B156" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.45">
@@ -2334,7 +2357,7 @@
         <v>97</v>
       </c>
       <c r="B157" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.45">
@@ -2342,7 +2365,7 @@
         <v>97</v>
       </c>
       <c r="B158" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.45">
@@ -2350,7 +2373,7 @@
         <v>97</v>
       </c>
       <c r="B159" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.45">
@@ -2358,7 +2381,7 @@
         <v>97</v>
       </c>
       <c r="B160" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.45">
@@ -2366,7 +2389,7 @@
         <v>97</v>
       </c>
       <c r="B161" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.45">
@@ -2374,7 +2397,7 @@
         <v>97</v>
       </c>
       <c r="B162" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.45">
@@ -2382,7 +2405,7 @@
         <v>97</v>
       </c>
       <c r="B163" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.45">
@@ -2390,7 +2413,7 @@
         <v>97</v>
       </c>
       <c r="B164" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.45">
@@ -2398,7 +2421,7 @@
         <v>97</v>
       </c>
       <c r="B165" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.45">
@@ -2406,7 +2429,7 @@
         <v>97</v>
       </c>
       <c r="B166" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.45">
@@ -2414,7 +2437,7 @@
         <v>97</v>
       </c>
       <c r="B167" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.45">
@@ -2422,7 +2445,7 @@
         <v>97</v>
       </c>
       <c r="B168" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.45">
@@ -2430,7 +2453,7 @@
         <v>97</v>
       </c>
       <c r="B169" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.45">
@@ -2438,7 +2461,7 @@
         <v>97</v>
       </c>
       <c r="B170" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.45">
@@ -2446,7 +2469,7 @@
         <v>97</v>
       </c>
       <c r="B171" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.45">
@@ -2454,7 +2477,7 @@
         <v>97</v>
       </c>
       <c r="B172" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.45">
@@ -2462,7 +2485,7 @@
         <v>97</v>
       </c>
       <c r="B173" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.45">
@@ -2470,7 +2493,7 @@
         <v>97</v>
       </c>
       <c r="B174" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.45">
@@ -2478,7 +2501,7 @@
         <v>97</v>
       </c>
       <c r="B175" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.45">
@@ -2486,7 +2509,7 @@
         <v>97</v>
       </c>
       <c r="B176" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.45">
@@ -2494,7 +2517,7 @@
         <v>97</v>
       </c>
       <c r="B177" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.45">
@@ -2502,7 +2525,7 @@
         <v>97</v>
       </c>
       <c r="B178" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.45">
@@ -2510,7 +2533,7 @@
         <v>97</v>
       </c>
       <c r="B179" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.45">
@@ -2518,7 +2541,7 @@
         <v>97</v>
       </c>
       <c r="B180" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.45">
@@ -2526,7 +2549,7 @@
         <v>97</v>
       </c>
       <c r="B181" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.45">
@@ -2534,7 +2557,7 @@
         <v>97</v>
       </c>
       <c r="B182" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.45">
@@ -2542,7 +2565,7 @@
         <v>97</v>
       </c>
       <c r="B183" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.45">
@@ -2550,7 +2573,7 @@
         <v>97</v>
       </c>
       <c r="B184" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.45">
@@ -2558,7 +2581,7 @@
         <v>97</v>
       </c>
       <c r="B185" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.45">
@@ -2566,7 +2589,7 @@
         <v>97</v>
       </c>
       <c r="B186" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.45">
@@ -2574,7 +2597,7 @@
         <v>97</v>
       </c>
       <c r="B187" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.45">
@@ -2582,7 +2605,7 @@
         <v>97</v>
       </c>
       <c r="B188" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.45">
@@ -2590,7 +2613,7 @@
         <v>97</v>
       </c>
       <c r="B189" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.45">
@@ -2598,7 +2621,7 @@
         <v>97</v>
       </c>
       <c r="B190" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.45">
@@ -2606,7 +2629,7 @@
         <v>97</v>
       </c>
       <c r="B191" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.45">
@@ -2614,7 +2637,7 @@
         <v>97</v>
       </c>
       <c r="B192" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.45">
@@ -2622,7 +2645,7 @@
         <v>97</v>
       </c>
       <c r="B193" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.45">
@@ -2630,7 +2653,7 @@
         <v>97</v>
       </c>
       <c r="B194" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.45">
@@ -2638,7 +2661,7 @@
         <v>97</v>
       </c>
       <c r="B195" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.45">
@@ -2646,7 +2669,7 @@
         <v>97</v>
       </c>
       <c r="B196" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.45">
@@ -2654,7 +2677,7 @@
         <v>97</v>
       </c>
       <c r="B197" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.45">
@@ -2662,7 +2685,7 @@
         <v>97</v>
       </c>
       <c r="B198" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.45">
@@ -2670,7 +2693,7 @@
         <v>97</v>
       </c>
       <c r="B199" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.45">
@@ -2678,7 +2701,7 @@
         <v>97</v>
       </c>
       <c r="B200" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.45">
@@ -2686,7 +2709,7 @@
         <v>97</v>
       </c>
       <c r="B201" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.45">
@@ -2694,7 +2717,7 @@
         <v>97</v>
       </c>
       <c r="B202" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.45">
@@ -2702,7 +2725,7 @@
         <v>97</v>
       </c>
       <c r="B203" t="s">
-        <v>219</v>
+        <v>80</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.45">
@@ -2710,7 +2733,7 @@
         <v>97</v>
       </c>
       <c r="B204" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.45">
@@ -2718,15 +2741,15 @@
         <v>97</v>
       </c>
       <c r="B205" t="s">
-        <v>83</v>
+        <v>219</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A206" t="s">
         <v>97</v>
       </c>
-      <c r="B206" t="s">
-        <v>84</v>
+      <c r="B206" s="2" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.45">
@@ -2734,7 +2757,7 @@
         <v>97</v>
       </c>
       <c r="B207" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.45">
@@ -2742,7 +2765,7 @@
         <v>97</v>
       </c>
       <c r="B208" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.45">
@@ -2750,7 +2773,7 @@
         <v>97</v>
       </c>
       <c r="B209" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.45">
@@ -2758,7 +2781,7 @@
         <v>97</v>
       </c>
       <c r="B210" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.45">
@@ -2766,7 +2789,7 @@
         <v>97</v>
       </c>
       <c r="B211" t="s">
-        <v>89</v>
+        <v>222</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.45">
@@ -2774,7 +2797,7 @@
         <v>97</v>
       </c>
       <c r="B212" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.45">
@@ -2782,7 +2805,7 @@
         <v>97</v>
       </c>
       <c r="B213" t="s">
-        <v>220</v>
+        <v>87</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.45">
@@ -2790,7 +2813,7 @@
         <v>97</v>
       </c>
       <c r="B214" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.45">
@@ -2798,7 +2821,7 @@
         <v>97</v>
       </c>
       <c r="B215" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.45">
@@ -2806,7 +2829,7 @@
         <v>97</v>
       </c>
       <c r="B216" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.45">
@@ -2814,7 +2837,7 @@
         <v>97</v>
       </c>
       <c r="B217" t="s">
-        <v>94</v>
+        <v>220</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.45">
@@ -2822,7 +2845,7 @@
         <v>97</v>
       </c>
       <c r="B218" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.45">
@@ -2830,7 +2853,7 @@
         <v>97</v>
       </c>
       <c r="B219" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.45">
@@ -2838,25 +2861,41 @@
         <v>97</v>
       </c>
       <c r="B220" t="s">
-        <v>222</v>
+        <v>93</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A221" t="s">
         <v>97</v>
       </c>
-      <c r="B221" s="2" t="s">
-        <v>223</v>
+      <c r="B221" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A222" t="s">
+        <v>97</v>
+      </c>
+      <c r="B222" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A223" t="s">
+        <v>97</v>
+      </c>
+      <c r="B223" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B220" xr:uid="{50C14BDF-EED2-4551-A2A9-086DD03AE42C}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B219">
-    <sortCondition ref="A2:A219"/>
-    <sortCondition ref="B2:B219"/>
+  <autoFilter ref="A1:B221" xr:uid="{50C14BDF-EED2-4551-A2A9-086DD03AE42C}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C223">
+    <sortCondition ref="A2:A223"/>
+    <sortCondition ref="B2:B223"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="B221" r:id="rId1" xr:uid="{F8843DE9-B4B0-4B94-B678-2704C55325B6}"/>
+    <hyperlink ref="B206" r:id="rId1" xr:uid="{F8843DE9-B4B0-4B94-B678-2704C55325B6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>